<commit_message>
Updated statistical analysis, updated supplemental figures
</commit_message>
<xml_diff>
--- a/Data/NAC/MotorBehaviordata_NAC_Livia022924.xlsx
+++ b/Data/NAC/MotorBehaviordata_NAC_Livia022924.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livia\Documents\Data Mito\data\raw\NAC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiaoguienko/git/LHMorais2024/Data/NAC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF105C90-A196-47FB-85BA-C48E0B2304E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3A904C-0106-1E43-AC9F-D730A6D3B2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{14CC993E-0CDB-4C1F-BA41-A215F3DE6160}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17120" windowHeight="15720" activeTab="1" xr2:uid="{14CC993E-0CDB-4C1F-BA41-A215F3DE6160}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -222,9 +222,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -262,7 +262,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -368,7 +368,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -510,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,28 +524,28 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -565,7 +565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -573,32 +573,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -606,7 +606,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -623,16 +623,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6AB8CE-CDE7-4CC0-B7A8-69D07539B035}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="M1" activeCellId="1" sqref="I1:I1048576 M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="144" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -667,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>111221</v>
       </c>
@@ -702,7 +702,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>111221</v>
       </c>
@@ -737,7 +737,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>111221</v>
       </c>
@@ -772,7 +772,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>111221</v>
       </c>
@@ -807,7 +807,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>111221</v>
       </c>
@@ -842,7 +842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>111221</v>
       </c>
@@ -877,7 +877,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>111221</v>
       </c>
@@ -912,7 +912,7 @@
         <v>14.78</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>111221</v>
       </c>
@@ -947,7 +947,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>111221</v>
       </c>
@@ -982,7 +982,7 @@
         <v>14.57</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>111221</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>111221</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>111221</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>5.93</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>111221</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>111221</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>5.73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>111221</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>5.37</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>111221</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>7.02</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>111221</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>111221</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>111221</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>111221</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>111221</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>6.48</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>111221</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>111221</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>8.17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>111221</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>10.18</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>111221</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>12.32</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>111221</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>111221</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>111221</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>111221</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>111221</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>111221</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>111221</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2182022</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>3.02</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2182022</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>4.01</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2182022</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>7.53</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2182022</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2182022</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>26.56</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2182022</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
         <v>33</v>
@@ -1997,7 +1997,7 @@
         <v>24.15</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2182022</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>17.149999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2182022</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>8.94</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2182022</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2182022</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2182022</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>31.57</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2182022</v>
       </c>
@@ -2207,85 +2207,85 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
     </row>
   </sheetData>

</xml_diff>